<commit_message>
Final code updates and adding docs for how to build
</commit_message>
<xml_diff>
--- a/circuit.xlsx
+++ b/circuit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The-Jabberwock\Documents\Code\arduino\synthetic_window\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D567CF85-914A-452D-89AA-9CE2F8B21150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C53D5F3-95B1-43FC-B6E9-EC8DB1698F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A04A8099-3290-4E50-9EFD-23D4CA440128}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>A</t>
   </si>
@@ -89,27 +89,6 @@
     <t>Q</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -141,9 +120,6 @@
   </si>
   <si>
     <t>A5</t>
-  </si>
-  <si>
-    <t>5V</t>
   </si>
   <si>
     <t>RST</t>
@@ -189,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +183,13 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="0.79998168889431442"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -286,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -488,38 +471,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
       <top style="thin">
         <color theme="0"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -533,30 +492,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0"/>
       </left>
       <right style="thin">
@@ -791,6 +726,43 @@
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -814,9 +786,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -832,9 +801,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -856,21 +822,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -880,25 +834,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -918,7 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -933,15 +875,115 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -954,111 +996,43 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1395,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C7FCB2-C0A7-4776-8060-7D294BED0FB6}">
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD19" sqref="AD19"/>
+      <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,7 +1380,7 @@
     <col min="1" max="19" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>1</v>
@@ -1463,630 +1437,613 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="86"/>
-      <c r="W2" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" s="20"/>
-    </row>
-    <row r="3" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="66"/>
+      <c r="W2" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="71"/>
+    </row>
+    <row r="3" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>24</v>
+      <c r="B3" s="91"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="18"/>
-      <c r="W3" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="X3" s="22"/>
-    </row>
-    <row r="4" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="16"/>
+      <c r="W3" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="73"/>
+    </row>
+    <row r="4" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="89" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="39"/>
-      <c r="W4" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="X4" s="48"/>
-    </row>
-    <row r="5" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="62"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="29"/>
+      <c r="W4" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="X4" s="75"/>
+    </row>
+    <row r="5" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="40"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="88"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="68"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="60"/>
-    </row>
-    <row r="6" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="52"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="41"/>
+    </row>
+    <row r="6" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="59"/>
-    </row>
-    <row r="7" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="40"/>
+    </row>
+    <row r="7" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="65"/>
-      <c r="S7" s="61"/>
-      <c r="W7" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="X7" s="51"/>
-    </row>
-    <row r="8" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="30"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="42"/>
+      <c r="W7" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="77"/>
+    </row>
+    <row r="8" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="90" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="88"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="38"/>
-      <c r="W8" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="X8" s="53"/>
-    </row>
-    <row r="9" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C8" s="68"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="28"/>
+      <c r="W8" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="X8" s="79"/>
+    </row>
+    <row r="9" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="13" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="83"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" s="8">
+      <c r="L9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="7">
         <v>3.3</v>
       </c>
-      <c r="S9" s="16"/>
-    </row>
-    <row r="10" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S9" s="14"/>
+    </row>
+    <row r="10" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="83"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="83"/>
-      <c r="R10" s="83"/>
-      <c r="S10" s="87"/>
-    </row>
-    <row r="11" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="57"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="67"/>
+    </row>
+    <row r="11" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="71"/>
-      <c r="P11" s="71"/>
-      <c r="Q11" s="71"/>
-      <c r="R11" s="71"/>
-      <c r="S11" s="77"/>
-      <c r="AB11" s="81"/>
-    </row>
-    <row r="12" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="57"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="58"/>
+    </row>
+    <row r="12" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="76"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="77"/>
-    </row>
-    <row r="13" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="57"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="85"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="58"/>
+    </row>
+    <row r="13" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="73"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="54"/>
       <c r="I13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="J13" s="37"/>
+      <c r="K13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N13" s="82"/>
-      <c r="O13" s="71"/>
-      <c r="P13" s="71"/>
-      <c r="Q13" s="71"/>
-      <c r="R13" s="71"/>
-      <c r="S13" s="77"/>
-    </row>
-    <row r="14" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="N13" s="62"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="58"/>
+    </row>
+    <row r="14" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="82"/>
-      <c r="O14" s="71"/>
-      <c r="P14" s="71"/>
-      <c r="Q14" s="71"/>
-      <c r="R14" s="71"/>
-      <c r="S14" s="77"/>
-    </row>
-    <row r="15" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="57"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="58"/>
+    </row>
+    <row r="15" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="71"/>
-      <c r="P15" s="71"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="71"/>
-      <c r="S15" s="77"/>
-    </row>
-    <row r="16" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="57"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="58"/>
+    </row>
+    <row r="16" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="82"/>
-      <c r="O16" s="71"/>
-      <c r="P16" s="71"/>
-      <c r="Q16" s="71"/>
-      <c r="R16" s="71"/>
-      <c r="S16" s="77"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="52"/>
+      <c r="S16" s="58"/>
     </row>
     <row r="17" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="71"/>
-      <c r="P17" s="71"/>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="71"/>
-      <c r="S17" s="77"/>
-      <c r="T17" s="70"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="51"/>
     </row>
     <row r="18" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="71"/>
-      <c r="O18" s="71"/>
-      <c r="P18" s="71"/>
-      <c r="Q18" s="71"/>
-      <c r="R18" s="71"/>
-      <c r="S18" s="77"/>
-      <c r="Y18" s="54"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="58"/>
+      <c r="Y18" s="38"/>
     </row>
     <row r="19" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="71"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="71"/>
-      <c r="N19" s="71"/>
-      <c r="O19" s="71"/>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="71"/>
-      <c r="R19" s="71"/>
-      <c r="S19" s="77"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="58"/>
     </row>
     <row r="20" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="71"/>
-      <c r="M20" s="71"/>
-      <c r="N20" s="71"/>
-      <c r="O20" s="71"/>
-      <c r="P20" s="71"/>
-      <c r="Q20" s="71"/>
-      <c r="R20" s="71"/>
-      <c r="S20" s="77"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="52"/>
+      <c r="P20" s="52"/>
+      <c r="Q20" s="52"/>
+      <c r="R20" s="52"/>
+      <c r="S20" s="58"/>
     </row>
     <row r="21" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="71"/>
-      <c r="O21" s="71"/>
-      <c r="P21" s="71"/>
-      <c r="Q21" s="71"/>
-      <c r="R21" s="71"/>
-      <c r="S21" s="77"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="58"/>
     </row>
     <row r="22" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
-      <c r="Q22" s="71"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="77"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="52"/>
+      <c r="S22" s="58"/>
     </row>
     <row r="23" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="71"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="71"/>
-      <c r="O23" s="71"/>
-      <c r="P23" s="71"/>
-      <c r="Q23" s="71"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="77"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="52"/>
+      <c r="S23" s="58"/>
     </row>
     <row r="24" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="71"/>
-      <c r="N24" s="71"/>
-      <c r="O24" s="71"/>
-      <c r="P24" s="71"/>
-      <c r="Q24" s="71"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="77"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="52"/>
+      <c r="S24" s="58"/>
     </row>
     <row r="25" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="78"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="79"/>
-      <c r="O25" s="79"/>
-      <c r="P25" s="79"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="79"/>
-      <c r="S25" s="80"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>